<commit_message>
changed aggregation of database. electricity split into 3 commodities
</commit_message>
<xml_diff>
--- a/support/aggregations/raw_to_aggregated.xlsx
+++ b/support/aggregations/raw_to_aggregated.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10751229_polimi_it/Documents/PhD/7_MSc_THESIS/Lorenzo_ROSSI/model/aggregations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzorinaldi/Documents/GitHub/SESAM/ExioSteel/support/aggregations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_F98CB395415A4E194524F6EFB611C8265FB1C824" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8B7691E-0D45-DD4A-ACD9-7C6F959A338C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD73AB6F-D5B8-C142-8F2A-A45582394341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="760" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9240" yWindow="-28800" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="777">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="779">
   <si>
     <t>Aggregation</t>
   </si>
@@ -2328,9 +2328,6 @@
     <t>WM</t>
   </si>
   <si>
-    <t>Electricity</t>
-  </si>
-  <si>
     <t>Coal</t>
   </si>
   <si>
@@ -2356,6 +2353,15 @@
   </si>
   <si>
     <t>Other Renewables</t>
+  </si>
+  <si>
+    <t>Electricity, fossil</t>
+  </si>
+  <si>
+    <t>Electricity, nuclear</t>
+  </si>
+  <si>
+    <t>Electricity, renewable</t>
   </si>
 </sst>
 </file>
@@ -2725,12 +2731,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A82" zoomScale="206" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97:B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="104.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3219,7 +3226,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
@@ -3227,7 +3234,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
@@ -3235,7 +3242,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
@@ -3243,7 +3250,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
@@ -3251,7 +3258,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
@@ -3259,7 +3266,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
@@ -3267,7 +3274,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
@@ -3275,7 +3282,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
@@ -3283,7 +3290,7 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
@@ -3291,7 +3298,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
@@ -3299,7 +3306,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
@@ -3307,7 +3314,7 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
@@ -3604,13 +3611,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B129" sqref="A129:B140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="110.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -4258,7 +4266,7 @@
         <v>284</v>
       </c>
       <c r="B129" t="s">
-        <v>767</v>
+        <v>776</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
@@ -4266,7 +4274,7 @@
         <v>285</v>
       </c>
       <c r="B130" t="s">
-        <v>767</v>
+        <v>776</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
@@ -4274,7 +4282,7 @@
         <v>286</v>
       </c>
       <c r="B131" t="s">
-        <v>767</v>
+        <v>777</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
@@ -4282,7 +4290,7 @@
         <v>287</v>
       </c>
       <c r="B132" t="s">
-        <v>767</v>
+        <v>778</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
@@ -4290,7 +4298,7 @@
         <v>288</v>
       </c>
       <c r="B133" t="s">
-        <v>767</v>
+        <v>778</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
@@ -4298,7 +4306,7 @@
         <v>289</v>
       </c>
       <c r="B134" t="s">
-        <v>767</v>
+        <v>776</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
@@ -4306,7 +4314,7 @@
         <v>290</v>
       </c>
       <c r="B135" t="s">
-        <v>767</v>
+        <v>778</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
@@ -4314,7 +4322,7 @@
         <v>291</v>
       </c>
       <c r="B136" t="s">
-        <v>767</v>
+        <v>778</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
@@ -4322,7 +4330,7 @@
         <v>292</v>
       </c>
       <c r="B137" t="s">
-        <v>767</v>
+        <v>778</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
@@ -4330,7 +4338,7 @@
         <v>293</v>
       </c>
       <c r="B138" t="s">
-        <v>767</v>
+        <v>778</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
@@ -4338,7 +4346,7 @@
         <v>294</v>
       </c>
       <c r="B139" t="s">
-        <v>767</v>
+        <v>778</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
@@ -4346,7 +4354,7 @@
         <v>295</v>
       </c>
       <c r="B140" t="s">
-        <v>767</v>
+        <v>776</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
changed aggregation of electricity commodities and added new steel techs
</commit_message>
<xml_diff>
--- a/support/aggregations/raw_to_aggregated.xlsx
+++ b/support/aggregations/raw_to_aggregated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzorinaldi/Documents/GitHub/SESAM/ExioSteel/support/aggregations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD73AB6F-D5B8-C142-8F2A-A45582394341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E43B1A3-08E3-B34F-B95F-F9AF6CECA0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-9240" yWindow="-28800" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="779">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="777">
   <si>
     <t>Aggregation</t>
   </si>
@@ -2355,13 +2355,7 @@
     <t>Other Renewables</t>
   </si>
   <si>
-    <t>Electricity, fossil</t>
-  </si>
-  <si>
-    <t>Electricity, nuclear</t>
-  </si>
-  <si>
-    <t>Electricity, renewable</t>
+    <t>Electricity</t>
   </si>
 </sst>
 </file>
@@ -3612,7 +3606,7 @@
   <dimension ref="A1:B201"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A118" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B129" sqref="A129:B140"/>
+      <selection activeCell="B129" sqref="B129:B140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4282,7 +4276,7 @@
         <v>286</v>
       </c>
       <c r="B131" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
@@ -4290,7 +4284,7 @@
         <v>287</v>
       </c>
       <c r="B132" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
@@ -4298,7 +4292,7 @@
         <v>288</v>
       </c>
       <c r="B133" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
@@ -4314,7 +4308,7 @@
         <v>290</v>
       </c>
       <c r="B135" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
@@ -4322,7 +4316,7 @@
         <v>291</v>
       </c>
       <c r="B136" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
@@ -4330,7 +4324,7 @@
         <v>292</v>
       </c>
       <c r="B137" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
@@ -4338,7 +4332,7 @@
         <v>293</v>
       </c>
       <c r="B138" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
@@ -4346,7 +4340,7 @@
         <v>294</v>
       </c>
       <c r="B139" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
db_building updated to consider ee mixes on the use side and keep electricity commodities disaggregated
</commit_message>
<xml_diff>
--- a/support/aggregations/raw_to_aggregated.xlsx
+++ b/support/aggregations/raw_to_aggregated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzorinaldi/Documents/GitHub/SESAM/ExioSteel/support/aggregations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E43B1A3-08E3-B34F-B95F-F9AF6CECA0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E469F5DC-FE10-094C-AA2B-A085E98C8272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-9240" yWindow="-28800" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="777">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="776">
   <si>
     <t>Aggregation</t>
   </si>
@@ -2353,9 +2353,6 @@
   </si>
   <si>
     <t>Other Renewables</t>
-  </si>
-  <si>
-    <t>Electricity</t>
   </si>
 </sst>
 </file>
@@ -3606,7 +3603,7 @@
   <dimension ref="A1:B201"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A118" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B129" sqref="B129:B140"/>
+      <selection activeCell="B140" sqref="B129:B140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4260,7 +4257,7 @@
         <v>284</v>
       </c>
       <c r="B129" t="s">
-        <v>776</v>
+        <v>767</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
@@ -4268,7 +4265,7 @@
         <v>285</v>
       </c>
       <c r="B130" t="s">
-        <v>776</v>
+        <v>768</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
@@ -4276,7 +4273,7 @@
         <v>286</v>
       </c>
       <c r="B131" t="s">
-        <v>776</v>
+        <v>769</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
@@ -4284,7 +4281,7 @@
         <v>287</v>
       </c>
       <c r="B132" t="s">
-        <v>776</v>
+        <v>770</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
@@ -4292,7 +4289,7 @@
         <v>288</v>
       </c>
       <c r="B133" t="s">
-        <v>776</v>
+        <v>771</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
@@ -4300,7 +4297,7 @@
         <v>289</v>
       </c>
       <c r="B134" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
@@ -4308,7 +4305,7 @@
         <v>290</v>
       </c>
       <c r="B135" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
@@ -4316,7 +4313,7 @@
         <v>291</v>
       </c>
       <c r="B136" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
@@ -4324,7 +4321,7 @@
         <v>292</v>
       </c>
       <c r="B137" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
@@ -4332,7 +4329,7 @@
         <v>293</v>
       </c>
       <c r="B138" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
@@ -4340,7 +4337,7 @@
         <v>294</v>
       </c>
       <c r="B139" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
@@ -4348,7 +4345,7 @@
         <v>295</v>
       </c>
       <c r="B140" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>